<commit_message>
fix: Arjun's xlsx files
</commit_message>
<xml_diff>
--- a/prisma/ArjunData/20230319_MM_folders/19th Century Composers/Czerny/Keyboard/Piano Etudes.xlsx
+++ b/prisma/ArjunData/20230319_MM_folders/19th Century Composers/Czerny/Keyboard/Piano Etudes.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -645,51 +645,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -705,20 +705,126 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J65" activeCellId="0" sqref="J65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +884,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -860,7 +966,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -980,7 +1086,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1020,7 +1126,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1060,7 +1166,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1100,7 +1206,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1140,7 +1246,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1180,7 +1286,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1220,7 +1326,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1260,7 +1366,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1340,7 +1446,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1460,7 +1566,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1500,7 +1606,7 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1620,7 +1726,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1660,7 +1766,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1702,7 +1808,7 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1742,7 +1848,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1782,7 +1888,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1944,7 +2050,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1984,7 +2090,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2024,7 +2130,7 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2066,7 +2172,7 @@
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2106,7 +2212,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2146,7 +2252,7 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2186,7 +2292,7 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2266,7 +2372,7 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2306,7 +2412,7 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2346,7 +2452,7 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2388,7 +2494,7 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2428,7 +2534,7 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -2470,7 +2576,7 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2512,7 +2618,7 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2752,7 +2858,7 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2832,7 +2938,7 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2872,7 +2978,7 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2956,7 +3062,7 @@
       <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -3040,7 +3146,7 @@
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3080,7 +3186,7 @@
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -3164,7 +3270,7 @@
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -3206,7 +3312,7 @@
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3246,7 +3352,7 @@
       <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -3370,7 +3476,7 @@
       <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -3450,7 +3556,7 @@
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -3530,7 +3636,7 @@
       <c r="Y69" s="3"/>
       <c r="Z69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -3572,7 +3678,7 @@
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -3736,7 +3842,7 @@
       <c r="Y74" s="3"/>
       <c r="Z74" s="3"/>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -3860,7 +3966,7 @@
       <c r="Y77" s="3"/>
       <c r="Z77" s="3"/>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -3900,7 +4006,7 @@
       <c r="Y78" s="3"/>
       <c r="Z78" s="3"/>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -3984,7 +4090,7 @@
       <c r="Y80" s="3"/>
       <c r="Z80" s="3"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -4024,7 +4130,7 @@
       <c r="Y81" s="3"/>
       <c r="Z81" s="3"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -4066,7 +4172,7 @@
       <c r="Y82" s="3"/>
       <c r="Z82" s="3"/>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -4108,7 +4214,7 @@
       <c r="Y83" s="3"/>
       <c r="Z83" s="3"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>16</v>
       </c>
@@ -4135,10 +4241,9 @@
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
       <c r="N84" s="3"/>
-      <c r="O84" s="5" t="s">
+      <c r="P84" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
       <c r="S84" s="3"/>
@@ -4150,7 +4255,7 @@
       <c r="Y84" s="3"/>
       <c r="Z84" s="3"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -4190,7 +4295,7 @@
       <c r="Y85" s="3"/>
       <c r="Z85" s="3"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -4230,7 +4335,7 @@
       <c r="Y86" s="3"/>
       <c r="Z86" s="3"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -4270,7 +4375,7 @@
       <c r="Y87" s="3"/>
       <c r="Z87" s="3"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -4310,7 +4415,7 @@
       <c r="Y88" s="3"/>
       <c r="Z88" s="3"/>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -4352,7 +4457,7 @@
       <c r="Y89" s="3"/>
       <c r="Z89" s="3"/>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -29944,7 +30049,7 @@
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" display="https://ks4.imslp.info/files/imglnks/usimg/c/cf/IMSLP593590-PMLP3452-czerny_op299_diabelli_CzerDie_49124441X.pdf"/>
     <hyperlink ref="P43" r:id="rId2" display="https://ks4.imslp.info/files/imglnks/usimg/c/c0/IMSLP643373-PMLP177367-czerny_g.371.s_40_ta-gliche_Studien_auf_dem_Piano-Forte_mit_vorgeschriebenen_Wiederholungen_..._337tes_Werk-_etc_full.pdf"/>
-    <hyperlink ref="O84" r:id="rId3" display="https://ks.imslp.net/files/imglnks/usimg/2/2b/IMSLP582004-PMLP14384-czerny_365_bk_1.pdf"/>
+    <hyperlink ref="P84" r:id="rId3" display="https://ks.imslp.net/files/imglnks/usimg/2/2b/IMSLP582004-PMLP14384-czerny_365_bk_1.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>